<commit_message>
Update test design technic daongochuy.xlsx
</commit_message>
<xml_diff>
--- a/test design technic daongochuy.xlsx
+++ b/test design technic daongochuy.xlsx
@@ -994,7 +994,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="515">
   <si>
     <r>
       <t xml:space="preserve">Security Classification: </t>
@@ -2711,9 +2711,6 @@
     <t>đ5000</t>
   </si>
   <si>
-    <t>1, Select any product then check displaying of currency in ViewProduct screen</t>
-  </si>
-  <si>
     <t>Original Price from 1 to 999</t>
   </si>
   <si>
@@ -2945,6 +2942,60 @@
   </si>
   <si>
     <t>User clicks on "Back" button</t>
+  </si>
+  <si>
+    <t>Verify that first photo focused on in photolist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Back" button when focus on the first picture in ViewProduct screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Back" button when focus on the second picture in ViewProduct screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Next" button when focus on the last picture in ViewProduct screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Next" button when focus on the close-to-last picture in ViewProduct screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Next" button when focus on a picture in ViewProduct screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that "Back" button disabled </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that "Back" button available </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that "Next" button disabled </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the next photo onward focused </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the photo backward focused </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Users click on each photo on the photo list in ViewProduct screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that photo focused on the big photo frame </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the text "No Picture" display on the big frame  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">reload page to check if first photo on the big frame focused when loading page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reload page to check if first photo on the list focused when loading page </t>
+  </si>
+  <si>
+    <t>Verify that first photo focused on big photo frame</t>
   </si>
 </sst>
 </file>
@@ -3982,7 +4033,7 @@
     <xf numFmtId="166" fontId="56" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="57" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="268">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -4629,6 +4680,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="24" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -4650,9 +4704,6 @@
     <xf numFmtId="0" fontId="3" fillId="28" borderId="17" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="24" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -4733,6 +4784,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="27">
@@ -6526,8 +6580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.3"/>
@@ -6856,10 +6910,10 @@
         <v>422</v>
       </c>
       <c r="C19" s="52" t="s">
-        <v>426</v>
+        <v>453</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E19" s="54" t="s">
         <v>425</v>
@@ -6872,7 +6926,7 @@
     <row r="20" spans="1:9" s="45" customFormat="1">
       <c r="A20" s="168"/>
       <c r="B20" s="225" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C20" s="226"/>
       <c r="D20" s="226"/>
@@ -6888,16 +6942,16 @@
         <v>2</v>
       </c>
       <c r="B21" s="52" t="s">
+        <v>426</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>429</v>
+      </c>
+      <c r="D21" s="60" t="s">
         <v>427</v>
       </c>
-      <c r="C21" s="52" t="s">
-        <v>430</v>
-      </c>
-      <c r="D21" s="60" t="s">
+      <c r="E21" s="54" t="s">
         <v>428</v>
-      </c>
-      <c r="E21" s="54" t="s">
-        <v>429</v>
       </c>
       <c r="F21" s="52"/>
       <c r="G21" s="52"/>
@@ -6913,13 +6967,13 @@
         <v>424</v>
       </c>
       <c r="C22" s="52" t="s">
+        <v>430</v>
+      </c>
+      <c r="D22" s="60" t="s">
+        <v>427</v>
+      </c>
+      <c r="E22" s="54" t="s">
         <v>431</v>
-      </c>
-      <c r="D22" s="60" t="s">
-        <v>428</v>
-      </c>
-      <c r="E22" s="54" t="s">
-        <v>432</v>
       </c>
       <c r="F22" s="52"/>
       <c r="G22" s="52"/>
@@ -6929,7 +6983,7 @@
     <row r="23" spans="1:9" s="45" customFormat="1">
       <c r="A23" s="168"/>
       <c r="B23" s="225" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C23" s="226"/>
       <c r="D23" s="226"/>
@@ -6945,16 +6999,16 @@
         <v>4</v>
       </c>
       <c r="B24" s="52" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D24" s="54" t="s">
+        <v>434</v>
+      </c>
+      <c r="E24" s="54" t="s">
         <v>435</v>
-      </c>
-      <c r="E24" s="54" t="s">
-        <v>436</v>
       </c>
       <c r="F24" s="52"/>
       <c r="G24" s="52"/>
@@ -6967,16 +7021,16 @@
         <v>5</v>
       </c>
       <c r="B25" s="52" t="s">
+        <v>439</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>467</v>
+      </c>
+      <c r="D25" s="60" t="s">
+        <v>434</v>
+      </c>
+      <c r="E25" s="54" t="s">
         <v>440</v>
-      </c>
-      <c r="C25" s="52" t="s">
-        <v>468</v>
-      </c>
-      <c r="D25" s="60" t="s">
-        <v>435</v>
-      </c>
-      <c r="E25" s="54" t="s">
-        <v>441</v>
       </c>
       <c r="F25" s="52"/>
       <c r="G25" s="52"/>
@@ -6989,16 +7043,16 @@
         <v>6</v>
       </c>
       <c r="B26" s="52" t="s">
+        <v>433</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>436</v>
+      </c>
+      <c r="D26" s="60" t="s">
         <v>434</v>
       </c>
-      <c r="C26" s="52" t="s">
-        <v>437</v>
-      </c>
-      <c r="D26" s="60" t="s">
-        <v>435</v>
-      </c>
       <c r="E26" s="54" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F26" s="52"/>
       <c r="G26" s="52"/>
@@ -7008,7 +7062,7 @@
     <row r="27" spans="1:9" s="48" customFormat="1" ht="13.8">
       <c r="A27" s="168"/>
       <c r="B27" s="222" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C27" s="223"/>
       <c r="D27" s="223"/>
@@ -7027,13 +7081,13 @@
         <v>423</v>
       </c>
       <c r="C28" s="52" t="s">
+        <v>444</v>
+      </c>
+      <c r="D28" s="60" t="s">
         <v>445</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="E28" s="54" t="s">
         <v>446</v>
-      </c>
-      <c r="E28" s="54" t="s">
-        <v>447</v>
       </c>
       <c r="F28" s="52"/>
       <c r="G28" s="52"/>
@@ -7046,16 +7100,16 @@
         <v>8</v>
       </c>
       <c r="B29" s="62" t="s">
+        <v>447</v>
+      </c>
+      <c r="C29" s="62" t="s">
         <v>448</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="D29" s="62" t="s">
+        <v>445</v>
+      </c>
+      <c r="E29" s="62" t="s">
         <v>449</v>
-      </c>
-      <c r="D29" s="62" t="s">
-        <v>446</v>
-      </c>
-      <c r="E29" s="62" t="s">
-        <v>450</v>
       </c>
       <c r="F29" s="62"/>
       <c r="G29" s="62"/>
@@ -7068,16 +7122,16 @@
         <v>9</v>
       </c>
       <c r="B30" s="62" t="s">
+        <v>450</v>
+      </c>
+      <c r="C30" s="62" t="s">
         <v>451</v>
       </c>
-      <c r="C30" s="62" t="s">
+      <c r="D30" s="62" t="s">
+        <v>445</v>
+      </c>
+      <c r="E30" s="62" t="s">
         <v>452</v>
-      </c>
-      <c r="D30" s="62" t="s">
-        <v>446</v>
-      </c>
-      <c r="E30" s="62" t="s">
-        <v>453</v>
       </c>
       <c r="F30" s="62"/>
       <c r="G30" s="62"/>
@@ -7106,10 +7160,10 @@
         <v>422</v>
       </c>
       <c r="C32" s="52" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D32" s="53" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E32" s="54" t="s">
         <v>425</v>
@@ -7122,7 +7176,7 @@
     <row r="33" spans="1:9" s="48" customFormat="1" ht="13.8">
       <c r="A33" s="168"/>
       <c r="B33" s="225" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C33" s="226"/>
       <c r="D33" s="226"/>
@@ -7138,16 +7192,16 @@
         <v>11</v>
       </c>
       <c r="B34" s="52" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D34" s="60" t="s">
+        <v>427</v>
+      </c>
+      <c r="E34" s="54" t="s">
         <v>428</v>
-      </c>
-      <c r="E34" s="54" t="s">
-        <v>429</v>
       </c>
       <c r="F34" s="52"/>
       <c r="G34" s="52"/>
@@ -7160,16 +7214,16 @@
         <v>12</v>
       </c>
       <c r="B35" s="52" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C35" s="52" t="s">
+        <v>430</v>
+      </c>
+      <c r="D35" s="60" t="s">
+        <v>427</v>
+      </c>
+      <c r="E35" s="54" t="s">
         <v>431</v>
-      </c>
-      <c r="D35" s="60" t="s">
-        <v>428</v>
-      </c>
-      <c r="E35" s="54" t="s">
-        <v>432</v>
       </c>
       <c r="F35" s="52"/>
       <c r="G35" s="52"/>
@@ -7179,7 +7233,7 @@
     <row r="36" spans="1:9" s="48" customFormat="1" ht="13.8">
       <c r="A36" s="168"/>
       <c r="B36" s="225" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C36" s="226"/>
       <c r="D36" s="226"/>
@@ -7195,16 +7249,16 @@
         <v>13</v>
       </c>
       <c r="B37" s="52" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C37" s="52" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D37" s="54" t="s">
+        <v>434</v>
+      </c>
+      <c r="E37" s="54" t="s">
         <v>435</v>
-      </c>
-      <c r="E37" s="54" t="s">
-        <v>436</v>
       </c>
       <c r="F37" s="52"/>
       <c r="G37" s="52"/>
@@ -7217,16 +7271,16 @@
         <v>14</v>
       </c>
       <c r="B38" s="52" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C38" s="52" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D38" s="60" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E38" s="54" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F38" s="52"/>
       <c r="G38" s="52"/>
@@ -7239,16 +7293,16 @@
         <v>15</v>
       </c>
       <c r="B39" s="52" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C39" s="52" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D39" s="60" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E39" s="54" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F39" s="52"/>
       <c r="G39" s="52"/>
@@ -7258,7 +7312,7 @@
     <row r="40" spans="1:9" s="48" customFormat="1" ht="13.8">
       <c r="A40" s="168"/>
       <c r="B40" s="222" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C40" s="223"/>
       <c r="D40" s="223"/>
@@ -7274,16 +7328,16 @@
         <v>16</v>
       </c>
       <c r="B41" s="52" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C41" s="52" t="s">
+        <v>444</v>
+      </c>
+      <c r="D41" s="60" t="s">
         <v>445</v>
       </c>
-      <c r="D41" s="60" t="s">
+      <c r="E41" s="54" t="s">
         <v>446</v>
-      </c>
-      <c r="E41" s="54" t="s">
-        <v>447</v>
       </c>
       <c r="F41" s="52"/>
       <c r="G41" s="52"/>
@@ -7296,16 +7350,16 @@
         <v>17</v>
       </c>
       <c r="B42" s="62" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C42" s="62" t="s">
+        <v>448</v>
+      </c>
+      <c r="D42" s="62" t="s">
+        <v>445</v>
+      </c>
+      <c r="E42" s="62" t="s">
         <v>449</v>
-      </c>
-      <c r="D42" s="62" t="s">
-        <v>446</v>
-      </c>
-      <c r="E42" s="62" t="s">
-        <v>450</v>
       </c>
       <c r="F42" s="62"/>
       <c r="G42" s="62"/>
@@ -7318,16 +7372,16 @@
         <v>18</v>
       </c>
       <c r="B43" s="62" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C43" s="62" t="s">
+        <v>451</v>
+      </c>
+      <c r="D43" s="62" t="s">
+        <v>445</v>
+      </c>
+      <c r="E43" s="62" t="s">
         <v>452</v>
-      </c>
-      <c r="D43" s="62" t="s">
-        <v>446</v>
-      </c>
-      <c r="E43" s="62" t="s">
-        <v>453</v>
       </c>
       <c r="F43" s="62"/>
       <c r="G43" s="62"/>
@@ -7336,16 +7390,16 @@
     </row>
     <row r="44" spans="1:9" s="48" customFormat="1" ht="13.8">
       <c r="A44" s="168"/>
-      <c r="B44" s="232" t="s">
-        <v>463</v>
-      </c>
-      <c r="C44" s="233"/>
-      <c r="D44" s="233"/>
-      <c r="E44" s="233"/>
-      <c r="F44" s="233"/>
-      <c r="G44" s="233"/>
-      <c r="H44" s="233"/>
-      <c r="I44" s="234"/>
+      <c r="B44" s="233" t="s">
+        <v>462</v>
+      </c>
+      <c r="C44" s="234"/>
+      <c r="D44" s="234"/>
+      <c r="E44" s="234"/>
+      <c r="F44" s="234"/>
+      <c r="G44" s="234"/>
+      <c r="H44" s="234"/>
+      <c r="I44" s="235"/>
     </row>
     <row r="45" spans="1:9" s="48" customFormat="1" ht="13.8">
       <c r="A45" s="58">
@@ -7353,16 +7407,16 @@
         <v>19</v>
       </c>
       <c r="B45" s="62" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D45" s="62" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E45" s="62" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F45" s="62"/>
       <c r="G45" s="62"/>
@@ -7375,16 +7429,16 @@
         <v>20</v>
       </c>
       <c r="B46" s="52" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C46" s="62" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D46" s="60" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E46" s="54" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F46" s="52"/>
       <c r="G46" s="52"/>
@@ -7397,16 +7451,16 @@
         <v>21</v>
       </c>
       <c r="B47" s="52" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C47" s="62" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D47" s="60" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E47" s="54" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F47" s="52"/>
       <c r="G47" s="52"/>
@@ -7419,16 +7473,16 @@
         <v>22</v>
       </c>
       <c r="B48" s="52" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C48" s="62" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D48" s="60" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E48" s="54" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F48" s="52"/>
       <c r="G48" s="52"/>
@@ -7437,61 +7491,64 @@
     </row>
     <row r="49" spans="1:9" s="48" customFormat="1" ht="13.8">
       <c r="A49" s="167"/>
-      <c r="B49" s="235" t="s">
+      <c r="B49" s="236" t="s">
+        <v>480</v>
+      </c>
+      <c r="C49" s="237"/>
+      <c r="D49" s="237"/>
+      <c r="E49" s="237"/>
+      <c r="F49" s="237"/>
+      <c r="G49" s="237"/>
+      <c r="H49" s="237"/>
+      <c r="I49" s="237"/>
+    </row>
+    <row r="50" spans="1:9" s="48" customFormat="1" ht="13.8">
+      <c r="A50" s="180"/>
+      <c r="B50" s="238" t="s">
         <v>481</v>
       </c>
-      <c r="C49" s="236"/>
-      <c r="D49" s="236"/>
-      <c r="E49" s="236"/>
-      <c r="F49" s="236"/>
-      <c r="G49" s="236"/>
-      <c r="H49" s="236"/>
-      <c r="I49" s="236"/>
-    </row>
-    <row r="50" spans="1:9" s="48" customFormat="1" ht="13.8">
-      <c r="A50" s="179">
-        <f t="shared" ca="1" si="1"/>
+      <c r="C50" s="239"/>
+      <c r="D50" s="239"/>
+      <c r="E50" s="239"/>
+      <c r="F50" s="239"/>
+      <c r="G50" s="239"/>
+      <c r="H50" s="239"/>
+      <c r="I50" s="239"/>
+    </row>
+    <row r="51" spans="1:9" s="48" customFormat="1" ht="13.8">
+      <c r="A51" s="58">
         <v>23</v>
       </c>
-      <c r="B50" s="182" t="s">
-        <v>494</v>
-      </c>
-      <c r="C50" s="181"/>
-      <c r="D50" s="181"/>
-      <c r="E50" s="181"/>
-      <c r="F50" s="181"/>
-      <c r="G50" s="181"/>
-      <c r="H50" s="181"/>
-      <c r="I50" s="181"/>
-    </row>
-    <row r="51" spans="1:9" s="48" customFormat="1" ht="13.8">
-      <c r="A51" s="180"/>
-      <c r="B51" s="237" t="s">
+      <c r="B51" s="52" t="s">
         <v>482</v>
       </c>
-      <c r="C51" s="238"/>
-      <c r="D51" s="238"/>
-      <c r="E51" s="238"/>
-      <c r="F51" s="238"/>
-      <c r="G51" s="238"/>
-      <c r="H51" s="238"/>
-      <c r="I51" s="238"/>
+      <c r="C51" s="52"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="61"/>
     </row>
     <row r="52" spans="1:9" s="48" customFormat="1" ht="13.8">
-      <c r="A52" s="58">
+      <c r="A52" s="179">
         <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
-      <c r="B52" s="52" t="s">
-        <v>483</v>
-      </c>
-      <c r="C52" s="52"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="54"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="52"/>
-      <c r="I52" s="61"/>
+      <c r="B52" s="182" t="s">
+        <v>493</v>
+      </c>
+      <c r="C52" s="182" t="s">
+        <v>513</v>
+      </c>
+      <c r="D52" s="267" t="s">
+        <v>497</v>
+      </c>
+      <c r="E52" s="181"/>
+      <c r="F52" s="181"/>
+      <c r="G52" s="181"/>
+      <c r="H52" s="181"/>
+      <c r="I52" s="181"/>
     </row>
     <row r="53" spans="1:9" s="48" customFormat="1" ht="13.8">
       <c r="A53" s="58">
@@ -7499,7 +7556,7 @@
         <v>25</v>
       </c>
       <c r="B53" s="52" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C53" s="52"/>
       <c r="D53" s="60"/>
@@ -7515,7 +7572,7 @@
         <v>26</v>
       </c>
       <c r="B54" s="52" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C54" s="52"/>
       <c r="D54" s="60"/>
@@ -7531,7 +7588,7 @@
         <v>27</v>
       </c>
       <c r="B55" s="52" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C55" s="52"/>
       <c r="D55" s="60"/>
@@ -7547,7 +7604,7 @@
         <v>28</v>
       </c>
       <c r="B56" s="52" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C56" s="52"/>
       <c r="D56" s="60"/>
@@ -7559,8 +7616,8 @@
     </row>
     <row r="57" spans="1:9" s="48" customFormat="1" ht="13.8">
       <c r="A57" s="180"/>
-      <c r="B57" s="239" t="s">
-        <v>488</v>
+      <c r="B57" s="232" t="s">
+        <v>487</v>
       </c>
       <c r="C57" s="226"/>
       <c r="D57" s="226"/>
@@ -7576,10 +7633,14 @@
         <v>29</v>
       </c>
       <c r="B58" s="52" t="s">
-        <v>489</v>
-      </c>
-      <c r="C58" s="52"/>
-      <c r="D58" s="60"/>
+        <v>488</v>
+      </c>
+      <c r="C58" s="52" t="s">
+        <v>498</v>
+      </c>
+      <c r="D58" s="60" t="s">
+        <v>503</v>
+      </c>
       <c r="E58" s="54"/>
       <c r="F58" s="52"/>
       <c r="G58" s="52"/>
@@ -7592,10 +7653,14 @@
         <v>30</v>
       </c>
       <c r="B59" s="52" t="s">
-        <v>490</v>
-      </c>
-      <c r="C59" s="52"/>
-      <c r="D59" s="60"/>
+        <v>489</v>
+      </c>
+      <c r="C59" s="52" t="s">
+        <v>499</v>
+      </c>
+      <c r="D59" s="60" t="s">
+        <v>504</v>
+      </c>
       <c r="E59" s="54"/>
       <c r="F59" s="52"/>
       <c r="G59" s="52"/>
@@ -7608,10 +7673,14 @@
         <v>31</v>
       </c>
       <c r="B60" s="52" t="s">
-        <v>491</v>
-      </c>
-      <c r="C60" s="52"/>
-      <c r="D60" s="60"/>
+        <v>490</v>
+      </c>
+      <c r="C60" s="52" t="s">
+        <v>500</v>
+      </c>
+      <c r="D60" s="60" t="s">
+        <v>505</v>
+      </c>
       <c r="E60" s="54"/>
       <c r="F60" s="52"/>
       <c r="G60" s="52"/>
@@ -7624,10 +7693,14 @@
         <v>32</v>
       </c>
       <c r="B61" s="52" t="s">
-        <v>492</v>
-      </c>
-      <c r="C61" s="52"/>
-      <c r="D61" s="60"/>
+        <v>491</v>
+      </c>
+      <c r="C61" s="52" t="s">
+        <v>501</v>
+      </c>
+      <c r="D61" s="60" t="s">
+        <v>505</v>
+      </c>
       <c r="E61" s="54"/>
       <c r="F61" s="52"/>
       <c r="G61" s="52"/>
@@ -7636,14 +7709,18 @@
     </row>
     <row r="62" spans="1:9" s="48" customFormat="1" ht="13.8">
       <c r="A62" s="58">
-        <f t="shared" ref="A62:A66" ca="1" si="2">IF(OFFSET(A62,-1,0) ="",OFFSET(A62,-2,0)+1,OFFSET(A62,-1,0)+1 )</f>
+        <f t="shared" ref="A62:A67" ca="1" si="2">IF(OFFSET(A62,-1,0) ="",OFFSET(A62,-2,0)+1,OFFSET(A62,-1,0)+1 )</f>
         <v>33</v>
       </c>
       <c r="B62" s="52" t="s">
-        <v>496</v>
-      </c>
-      <c r="C62" s="52"/>
-      <c r="D62" s="53"/>
+        <v>495</v>
+      </c>
+      <c r="C62" s="52" t="s">
+        <v>502</v>
+      </c>
+      <c r="D62" s="53" t="s">
+        <v>506</v>
+      </c>
       <c r="E62" s="54"/>
       <c r="F62" s="52"/>
       <c r="G62" s="52"/>
@@ -7656,10 +7733,14 @@
         <v>34</v>
       </c>
       <c r="B63" s="52" t="s">
-        <v>497</v>
-      </c>
-      <c r="C63" s="52"/>
-      <c r="D63" s="54"/>
+        <v>496</v>
+      </c>
+      <c r="C63" s="52" t="s">
+        <v>502</v>
+      </c>
+      <c r="D63" s="54" t="s">
+        <v>507</v>
+      </c>
       <c r="E63" s="60"/>
       <c r="F63" s="52"/>
       <c r="G63" s="52"/>
@@ -7669,7 +7750,7 @@
     <row r="64" spans="1:9" s="48" customFormat="1" ht="13.8">
       <c r="A64" s="168"/>
       <c r="B64" s="228" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C64" s="229"/>
       <c r="D64" s="229"/>
@@ -7679,43 +7760,58 @@
       <c r="H64" s="229"/>
       <c r="I64" s="230"/>
     </row>
-    <row r="65" spans="1:9" s="48" customFormat="1" ht="13.8">
+    <row r="65" spans="1:9" s="48" customFormat="1" ht="24.6">
       <c r="A65" s="58">
         <f t="shared" ca="1" si="2"/>
         <v>35</v>
       </c>
       <c r="B65" s="170" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C65" s="170"/>
-      <c r="D65" s="53"/>
+      <c r="D65" s="53" t="s">
+        <v>510</v>
+      </c>
       <c r="E65" s="53"/>
       <c r="F65" s="170"/>
       <c r="G65" s="170"/>
       <c r="H65" s="170"/>
       <c r="I65" s="63"/>
     </row>
-    <row r="66" spans="1:9" s="48" customFormat="1" ht="13.8">
+    <row r="66" spans="1:9" s="48" customFormat="1" ht="24.6">
       <c r="A66" s="58">
         <f t="shared" ca="1" si="2"/>
         <v>36</v>
       </c>
       <c r="B66" s="170" t="s">
-        <v>495</v>
-      </c>
-      <c r="C66" s="170"/>
-      <c r="D66" s="59"/>
+        <v>494</v>
+      </c>
+      <c r="C66" s="170" t="s">
+        <v>508</v>
+      </c>
+      <c r="D66" s="59" t="s">
+        <v>509</v>
+      </c>
       <c r="E66" s="53"/>
       <c r="F66" s="170"/>
       <c r="G66" s="170"/>
       <c r="H66" s="170"/>
       <c r="I66" s="63"/>
     </row>
-    <row r="67" spans="1:9" s="48" customFormat="1" ht="13.8">
-      <c r="A67" s="58"/>
-      <c r="B67" s="170"/>
-      <c r="C67" s="170"/>
-      <c r="D67" s="53"/>
+    <row r="67" spans="1:9" s="48" customFormat="1" ht="24.6">
+      <c r="A67" s="58">
+        <f t="shared" ca="1" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="B67" s="170" t="s">
+        <v>511</v>
+      </c>
+      <c r="C67" s="170" t="s">
+        <v>512</v>
+      </c>
+      <c r="D67" s="53" t="s">
+        <v>514</v>
+      </c>
       <c r="E67" s="53"/>
       <c r="F67" s="170"/>
       <c r="G67" s="170"/>
@@ -8058,7 +8154,7 @@
     <mergeCell ref="B40:I40"/>
     <mergeCell ref="B44:I44"/>
     <mergeCell ref="B49:I49"/>
-    <mergeCell ref="B51:I51"/>
+    <mergeCell ref="B50:I50"/>
     <mergeCell ref="B20:I20"/>
     <mergeCell ref="B23:I23"/>
     <mergeCell ref="C3:D3"/>
@@ -8087,7 +8183,7 @@
       <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F86:H96 F37:H39 F65:H67 F72:H84 F28:H28 F19:H19 F21:H22 F24:H26 F41:H41 F32:H32 F34:H35 F46:H48 F52:H56 F58:H63">
+    <dataValidation type="list" allowBlank="1" sqref="F86:H96 F37:H39 F65:H67 F72:H84 F28:H28 F19:H19 F21:H22 F24:H26 F41:H41 F32:H32 F34:H35 F46:H48 F58:H63 F51:H51 F53:H56">
       <formula1>$A$11:$A$15</formula1>
     </dataValidation>
   </dataValidations>
@@ -13475,15 +13571,15 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E3E4FA-795A-4742-A021-9CDC3210C50B}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="044e8ed5-b60c-40cd-b477-04c240ccf9c3"/>
     <ds:schemaRef ds:uri="cabca498-5e2a-459c-ade0-601c6a98c846"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="044e8ed5-b60c-40cd-b477-04c240ccf9c3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>